<commit_message>
Updated parameters to give working simulation
</commit_message>
<xml_diff>
--- a/ADM1_input.xlsx
+++ b/ADM1_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tmlouw_sun_ac_za/Documents/Programming/MATLAB/ADM1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tmlouw_sun_ac_za/Documents/Programming/Git projects/Anaerobic-Digestion-Model-No.1-ADM1-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="13_ncr:1_{CF01C3F5-B680-4845-8933-33FC0021E36D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8A29A71B-69D1-43D7-8E8B-4411478BCA42}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="13_ncr:1_{CF01C3F5-B680-4845-8933-33FC0021E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209EFFDE-048A-471C-9566-160E6F275C97}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3A3FD143-C3DF-421E-A19F-87727448EE4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3A3FD143-C3DF-421E-A19F-87727448EE4D}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="SteadyStateOutputs" sheetId="2" r:id="rId3"/>
     <sheet name="Parameters" sheetId="3" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Parameters!$A$1:$E$102</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -417,6 +416,9 @@
     <t>KH.co2</t>
   </si>
   <si>
+    <t>M/bar</t>
+  </si>
+  <si>
     <t>KH.ch4</t>
   </si>
   <si>
@@ -426,6 +428,12 @@
     <t>Amb.R</t>
   </si>
   <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
     <t>Amb.P</t>
   </si>
   <si>
@@ -441,9 +449,15 @@
     <t>Process.KLA</t>
   </si>
   <si>
+    <t>1/d</t>
+  </si>
+  <si>
     <t>Process.Vl</t>
   </si>
   <si>
+    <t>m3</t>
+  </si>
+  <si>
     <t>Process.Vg</t>
   </si>
   <si>
@@ -453,6 +467,12 @@
     <t>m3/d</t>
   </si>
   <si>
+    <t>bar/M/K</t>
+  </si>
+  <si>
+    <t>m3/d/bar</t>
+  </si>
+  <si>
     <t>Fractionation constants</t>
   </si>
   <si>
@@ -607,27 +627,6 @@
   </si>
   <si>
     <t>Provides all parameters for ADM1, except the carbon content "Ci", which is defined in the code "funcADM1_ParameterSpec.m"</t>
-  </si>
-  <si>
-    <t>(M/bar)</t>
-  </si>
-  <si>
-    <t>(bar/M/K)</t>
-  </si>
-  <si>
-    <t>(bar)</t>
-  </si>
-  <si>
-    <t>(K)</t>
-  </si>
-  <si>
-    <t>(m3/d/bar)</t>
-  </si>
-  <si>
-    <t>(1/d)</t>
-  </si>
-  <si>
-    <t>(m3)</t>
   </si>
 </sst>
 </file>
@@ -680,11 +679,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,12 +1016,12 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1031,34 +1029,34 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1073,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B753A2-3EBF-459A-9A6B-36F0A48D4544}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1759,1477 +1757,1375 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C0FAE9-B51C-45AD-AC84-2DA9F0585241}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1">
         <v>0.95</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>0.23</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>0.13</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>0.26</v>
       </c>
       <c r="D4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>0.27</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>0.05</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>0.41</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>0.4</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>0.19</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>0.06</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11">
         <v>0.2</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
-      </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>0.2</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
-      </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>0.3</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>0.1</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>0.2</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>0.1</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>0.08</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <v>0.06</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>0.06</v>
       </c>
       <c r="D19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20">
         <v>0.04</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
-      </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21">
         <v>0.05</v>
       </c>
       <c r="D21" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22">
         <v>0.06</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23">
         <f>0.08/14</f>
         <v>5.7142857142857143E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
-      </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25">
         <f>0.0376/14</f>
         <v>2.6857142857142856E-3</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26">
         <f>0.06/14</f>
         <v>4.2857142857142859E-3</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27">
         <v>0.5</v>
       </c>
       <c r="D27" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
-      </c>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31">
         <v>0.02</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="3"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32">
         <v>0.02</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33">
         <v>0.02</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34">
         <v>0.02</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>151</v>
-      </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35">
         <v>0.02</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
-      </c>
-      <c r="F35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36">
         <v>0.02</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
-        <v>153</v>
-      </c>
-      <c r="F36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37">
         <v>0.02</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
-      </c>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38">
         <v>0.02</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
-        <v>150</v>
-      </c>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39">
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
-      </c>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40">
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E41" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42">
         <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E42" t="s">
-        <v>151</v>
-      </c>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43">
         <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44">
         <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E44" t="s">
-        <v>153</v>
-      </c>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E45" t="s">
-        <v>149</v>
-      </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46">
         <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E46" t="s">
-        <v>150</v>
-      </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="4">
+      <c r="B47">
         <v>0.5</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E47" t="s">
-        <v>154</v>
-      </c>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B48">
         <v>0.3</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
-      </c>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49">
         <v>0.4</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
-      </c>
-      <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B50">
         <v>0.2</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E50" t="s">
-        <v>151</v>
-      </c>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="4">
+      <c r="B51">
         <v>0.2</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E51" t="s">
-        <v>152</v>
-      </c>
-      <c r="F51" s="3"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52">
         <v>0.1</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E52" t="s">
-        <v>153</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B53">
         <v>0.15</v>
       </c>
       <c r="D53" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E53" t="s">
-        <v>149</v>
-      </c>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B54" s="3">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
-      </c>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B55">
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
-      </c>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B56">
         <v>4</v>
       </c>
       <c r="D56" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>92</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B57">
         <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E57" t="s">
-        <v>147</v>
-      </c>
-      <c r="F57" s="3"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B58">
         <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E58" t="s">
-        <v>151</v>
-      </c>
-      <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59">
         <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E59" t="s">
-        <v>152</v>
-      </c>
-      <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>98</v>
       </c>
-      <c r="B60" s="4">
+      <c r="B60">
         <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E60" t="s">
-        <v>153</v>
-      </c>
-      <c r="F60" s="3"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B61">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
-      </c>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="4">
+      <c r="B62">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>150</v>
-      </c>
-      <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B63">
         <v>5.5</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E63" t="s">
-        <v>154</v>
-      </c>
-      <c r="F63" s="3"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B64">
         <v>5.5</v>
       </c>
       <c r="D64" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E64" t="s">
-        <v>146</v>
-      </c>
-      <c r="F64" s="3"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65">
         <v>5.5</v>
       </c>
       <c r="D65" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E65" t="s">
-        <v>147</v>
-      </c>
-      <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>95</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B66">
         <v>5.5</v>
       </c>
       <c r="D66" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E66" t="s">
-        <v>151</v>
-      </c>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>97</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67">
         <v>5.5</v>
       </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E67" t="s">
-        <v>152</v>
-      </c>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B68">
         <v>5.5</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
-      </c>
-      <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69">
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E69" t="s">
-        <v>149</v>
-      </c>
-      <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>103</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B70">
         <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E70" t="s">
-        <v>150</v>
-      </c>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>104</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B71" s="3">
         <v>1E-4</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E71" t="s">
-        <v>154</v>
-      </c>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>105</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B72" s="3">
         <v>1E-4</v>
       </c>
       <c r="D72" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E72" t="s">
-        <v>146</v>
-      </c>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B73" s="3">
         <v>1E-4</v>
       </c>
       <c r="D73" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E73" t="s">
-        <v>147</v>
-      </c>
-      <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B74" s="3">
         <v>1E-4</v>
       </c>
       <c r="D74" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E74" t="s">
-        <v>151</v>
-      </c>
-      <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>108</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B75" s="3">
         <v>1E-4</v>
       </c>
       <c r="D75" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E75" t="s">
-        <v>152</v>
-      </c>
-      <c r="F75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>109</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B76" s="3">
         <v>1E-4</v>
       </c>
       <c r="D76" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E76" t="s">
-        <v>153</v>
-      </c>
-      <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B77" s="3">
         <v>1E-4</v>
       </c>
       <c r="D77" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E77" t="s">
-        <v>149</v>
-      </c>
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>111</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B78" s="3">
         <v>1E-4</v>
       </c>
       <c r="D78" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="E78" t="s">
-        <v>150</v>
-      </c>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>112</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B79" s="3">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="D79" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>147</v>
-      </c>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>113</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E80" t="s">
-        <v>151</v>
-      </c>
-      <c r="F80" s="3"/>
+        <v>158</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>114</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B81" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="D81" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E81" t="s">
-        <v>152</v>
-      </c>
-      <c r="F81" s="3"/>
+        <v>159</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>115</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82" s="3">
         <v>3.4999999999999999E-6</v>
       </c>
       <c r="D82" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="E82" t="s">
-        <v>153</v>
-      </c>
-      <c r="F82" s="3"/>
+        <v>160</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>116</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B83">
         <v>1.8E-3</v>
       </c>
       <c r="D83" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E83" t="s">
-        <v>149</v>
-      </c>
-      <c r="F83" s="3"/>
+        <v>156</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>117</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B84" s="3">
         <v>2.08E-14</v>
       </c>
       <c r="D84" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E84" t="s">
-        <v>159</v>
-      </c>
-      <c r="F84" s="3"/>
+        <v>166</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>118</v>
       </c>
-      <c r="B85" s="4">
-        <f>10^(-9.25)</f>
+      <c r="B85">
+        <f>10^-9.25</f>
         <v>5.6234132519034889E-10</v>
       </c>
       <c r="D85" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E85" t="s">
-        <v>160</v>
-      </c>
-      <c r="F85" s="3"/>
+        <v>167</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>119</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B86" s="3">
         <v>4.9399999999999995E-7</v>
       </c>
       <c r="D86" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E86" t="s">
-        <v>161</v>
-      </c>
-      <c r="F86" s="3"/>
+        <v>168</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>120</v>
       </c>
-      <c r="B87" s="4">
+      <c r="B87" s="3">
         <v>1.7399999999999999E-5</v>
       </c>
       <c r="D87" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E87" t="s">
-        <v>162</v>
-      </c>
-      <c r="F87" s="3"/>
+        <v>169</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>121</v>
       </c>
-      <c r="B88" s="4">
+      <c r="B88" s="3">
         <v>1.3200000000000001E-5</v>
       </c>
       <c r="D88" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E88" t="s">
-        <v>163</v>
-      </c>
-      <c r="F88" s="3"/>
+        <v>170</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>122</v>
       </c>
-      <c r="B89" s="4">
+      <c r="B89" s="3">
         <v>1.5E-5</v>
       </c>
       <c r="D89" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E89" t="s">
-        <v>164</v>
-      </c>
-      <c r="F89" s="3"/>
+        <v>171</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>123</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B90" s="3">
         <v>1.38E-5</v>
       </c>
       <c r="D90" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E90" t="s">
-        <v>148</v>
-      </c>
-      <c r="F90" s="3"/>
+        <v>155</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>124</v>
       </c>
-      <c r="B91" s="4">
+      <c r="B91">
         <v>2.7099999999999999E-2</v>
       </c>
-      <c r="C91" t="s">
-        <v>189</v>
-      </c>
       <c r="D91" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E91" t="s">
-        <v>166</v>
-      </c>
-      <c r="F91" s="3"/>
+        <v>173</v>
+      </c>
+      <c r="F91" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92">
+        <v>1.16E-3</v>
+      </c>
+      <c r="D92" t="s">
+        <v>172</v>
+      </c>
+      <c r="E92" t="s">
+        <v>174</v>
+      </c>
+      <c r="F92" t="s">
         <v>125</v>
       </c>
-      <c r="B92" s="4">
-        <v>1.16E-3</v>
-      </c>
-      <c r="C92" t="s">
-        <v>189</v>
-      </c>
-      <c r="D92" t="s">
-        <v>165</v>
-      </c>
-      <c r="E92" t="s">
-        <v>167</v>
-      </c>
-      <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>126</v>
-      </c>
-      <c r="B93" s="4">
+        <v>127</v>
+      </c>
+      <c r="B93" s="3">
         <v>7.3800000000000005E-4</v>
       </c>
-      <c r="C93" t="s">
-        <v>189</v>
-      </c>
       <c r="D93" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E93" t="s">
-        <v>168</v>
-      </c>
-      <c r="F93" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="F93" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>127</v>
-      </c>
-      <c r="B94" s="4">
+        <v>128</v>
+      </c>
+      <c r="B94">
         <v>8.3144999999999997E-2</v>
       </c>
-      <c r="C94" t="s">
-        <v>190</v>
-      </c>
       <c r="D94" t="s">
-        <v>169</v>
-      </c>
-      <c r="F94" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="F94" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>128</v>
-      </c>
-      <c r="B95" s="4">
+        <v>131</v>
+      </c>
+      <c r="B95">
         <v>1.0129999999999999</v>
       </c>
-      <c r="C95" t="s">
-        <v>191</v>
-      </c>
       <c r="D95" t="s">
-        <v>170</v>
-      </c>
-      <c r="F95" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="F95" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>129</v>
-      </c>
-      <c r="B96" s="4">
+        <v>132</v>
+      </c>
+      <c r="B96">
+        <f>35+273.15</f>
         <v>308.14999999999998</v>
       </c>
-      <c r="C96" t="s">
-        <v>192</v>
-      </c>
       <c r="D96" t="s">
-        <v>171</v>
-      </c>
-      <c r="F96" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="F96" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>130</v>
-      </c>
-      <c r="B97" s="4">
+        <v>133</v>
+      </c>
+      <c r="B97">
         <v>5.57E-2</v>
       </c>
-      <c r="C97" t="s">
-        <v>191</v>
-      </c>
       <c r="D97" t="s">
-        <v>172</v>
-      </c>
-      <c r="F97" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="F97" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>131</v>
-      </c>
-      <c r="B98" s="4">
+        <v>134</v>
+      </c>
+      <c r="B98" s="3">
         <v>50000</v>
       </c>
-      <c r="C98" t="s">
-        <v>193</v>
-      </c>
       <c r="D98" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="E98" t="s">
-        <v>174</v>
-      </c>
-      <c r="F98" s="3"/>
+        <v>181</v>
+      </c>
+      <c r="F98" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>132</v>
-      </c>
-      <c r="B99" s="4">
+        <v>135</v>
+      </c>
+      <c r="B99">
         <v>200</v>
       </c>
-      <c r="C99" t="s">
-        <v>194</v>
-      </c>
       <c r="D99" t="s">
-        <v>175</v>
-      </c>
-      <c r="F99" s="3"/>
+        <v>182</v>
+      </c>
+      <c r="F99" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>133</v>
-      </c>
-      <c r="B100" s="4">
+        <v>137</v>
+      </c>
+      <c r="B100">
         <v>3400</v>
       </c>
-      <c r="C100" t="s">
-        <v>195</v>
-      </c>
       <c r="D100" t="s">
-        <v>176</v>
-      </c>
-      <c r="F100" s="3"/>
+        <v>183</v>
+      </c>
+      <c r="F100" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>134</v>
-      </c>
-      <c r="B101" s="4">
+        <v>139</v>
+      </c>
+      <c r="B101">
         <v>100</v>
       </c>
-      <c r="C101" t="s">
-        <v>195</v>
-      </c>
       <c r="D101" t="s">
-        <v>177</v>
-      </c>
-      <c r="F101" s="3"/>
+        <v>184</v>
+      </c>
+      <c r="F101" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>135</v>
-      </c>
-      <c r="B102" s="4">
+        <v>140</v>
+      </c>
+      <c r="B102">
         <v>178.47</v>
       </c>
-      <c r="C102" t="s">
-        <v>136</v>
-      </c>
       <c r="D102" t="s">
-        <v>178</v>
-      </c>
-      <c r="F102" s="3"/>
+        <v>185</v>
+      </c>
+      <c r="F102" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E102" xr:uid="{6D163443-B0C1-4A57-B755-2044C62B5CBB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Excel file for BSM2_defaults for ease of use
</commit_message>
<xml_diff>
--- a/ADM1_input.xlsx
+++ b/ADM1_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stellenbosch-my.sharepoint.com/personal/tmlouw_sun_ac_za/Documents/Programming/Git projects/Anaerobic-Digestion-Model-No.1-ADM1-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="295" documentId="13_ncr:1_{CF01C3F5-B680-4845-8933-33FC0021E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209EFFDE-048A-471C-9566-160E6F275C97}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="13_ncr:1_{CF01C3F5-B680-4845-8933-33FC0021E36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89588C1C-117B-4517-ABA6-8302081EE5DF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3A3FD143-C3DF-421E-A19F-87727448EE4D}"/>
+    <workbookView xWindow="-135" yWindow="-16335" windowWidth="29070" windowHeight="15870" activeTab="3" xr2:uid="{3A3FD143-C3DF-421E-A19F-87727448EE4D}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="4" r:id="rId1"/>
@@ -1005,7 +1005,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1071,7 +1071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B753A2-3EBF-459A-9A6B-36F0A48D4544}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -1410,7 +1410,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1755,264 +1755,263 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C0FAE9-B51C-45AD-AC84-2DA9F0585241}">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>34</v>
       </c>
       <c r="B1">
         <v>0.95</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2">
         <v>0.23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
       <c r="B3">
         <v>0.13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4">
         <v>0.26</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5">
         <v>0.27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6">
         <v>0.05</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
       <c r="B7">
         <v>0.41</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
       <c r="B8">
         <v>0.4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>42</v>
       </c>
       <c r="B9">
         <v>0.19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10">
         <v>0.06</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
       <c r="B11">
         <v>0.2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
       <c r="B12">
         <v>0.2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
       <c r="B13">
         <v>0.3</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15">
         <v>0.2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
       <c r="B16">
         <v>0.1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
       <c r="B17">
         <v>0.08</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
       <c r="B18">
         <v>0.06</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
       <c r="B19">
         <v>0.06</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
       <c r="B20">
         <v>0.04</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
       <c r="B21">
         <v>0.05</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
       <c r="B22">
         <v>0.06</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -2020,22 +2019,22 @@
         <f>0.08/14</f>
         <v>5.7142857142857143E-3</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>57</v>
       </c>
       <c r="B24">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -2043,11 +2042,11 @@
         <f>0.0376/14</f>
         <v>2.6857142857142856E-3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2055,811 +2054,811 @@
         <f>0.06/14</f>
         <v>4.2857142857142859E-3</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>60</v>
       </c>
       <c r="B27">
         <v>0.5</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>61</v>
       </c>
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
       <c r="B30">
         <v>10</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>64</v>
       </c>
       <c r="B31">
         <v>0.02</v>
       </c>
+      <c r="C31" t="s">
+        <v>148</v>
+      </c>
       <c r="D31" t="s">
-        <v>148</v>
-      </c>
-      <c r="E31" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>65</v>
       </c>
       <c r="B32">
         <v>0.02</v>
       </c>
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
       <c r="D32" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>66</v>
       </c>
       <c r="B33">
         <v>0.02</v>
       </c>
+      <c r="C33" t="s">
+        <v>148</v>
+      </c>
       <c r="D33" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
       <c r="B34">
         <v>0.02</v>
       </c>
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
       <c r="D34" t="s">
-        <v>148</v>
-      </c>
-      <c r="E34" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>68</v>
       </c>
       <c r="B35">
         <v>0.02</v>
       </c>
+      <c r="C35" t="s">
+        <v>148</v>
+      </c>
       <c r="D35" t="s">
-        <v>148</v>
-      </c>
-      <c r="E35" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36">
         <v>0.02</v>
       </c>
+      <c r="C36" t="s">
+        <v>148</v>
+      </c>
       <c r="D36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E36" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
       <c r="B37">
         <v>0.02</v>
       </c>
+      <c r="C37" t="s">
+        <v>148</v>
+      </c>
       <c r="D37" t="s">
-        <v>148</v>
-      </c>
-      <c r="E37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
       <c r="B38">
         <v>0.02</v>
       </c>
+      <c r="C38" t="s">
+        <v>148</v>
+      </c>
       <c r="D38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>72</v>
       </c>
       <c r="B39">
         <v>30</v>
       </c>
+      <c r="C39" t="s">
+        <v>149</v>
+      </c>
       <c r="D39" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>73</v>
       </c>
       <c r="B40">
         <v>50</v>
       </c>
+      <c r="C40" t="s">
+        <v>149</v>
+      </c>
       <c r="D40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
       <c r="D41" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>75</v>
       </c>
       <c r="B42">
         <v>20</v>
       </c>
+      <c r="C42" t="s">
+        <v>149</v>
+      </c>
       <c r="D42" t="s">
-        <v>149</v>
-      </c>
-      <c r="E42" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>76</v>
       </c>
       <c r="B43">
         <v>20</v>
       </c>
+      <c r="C43" t="s">
+        <v>149</v>
+      </c>
       <c r="D43" t="s">
-        <v>149</v>
-      </c>
-      <c r="E43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>77</v>
       </c>
       <c r="B44">
         <v>13</v>
       </c>
+      <c r="C44" t="s">
+        <v>149</v>
+      </c>
       <c r="D44" t="s">
-        <v>149</v>
-      </c>
-      <c r="E44" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>78</v>
       </c>
       <c r="B45">
         <v>8</v>
       </c>
+      <c r="C45" t="s">
+        <v>149</v>
+      </c>
       <c r="D45" t="s">
-        <v>149</v>
-      </c>
-      <c r="E45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>79</v>
       </c>
       <c r="B46">
         <v>35</v>
       </c>
+      <c r="C46" t="s">
+        <v>149</v>
+      </c>
       <c r="D46" t="s">
-        <v>149</v>
-      </c>
-      <c r="E46" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>80</v>
       </c>
       <c r="B47">
         <v>0.5</v>
       </c>
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
       <c r="D47" t="s">
-        <v>150</v>
-      </c>
-      <c r="E47" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>81</v>
       </c>
       <c r="B48">
         <v>0.3</v>
       </c>
+      <c r="C48" t="s">
+        <v>150</v>
+      </c>
       <c r="D48" t="s">
-        <v>150</v>
-      </c>
-      <c r="E48" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>82</v>
       </c>
       <c r="B49">
         <v>0.4</v>
       </c>
+      <c r="C49" t="s">
+        <v>150</v>
+      </c>
       <c r="D49" t="s">
-        <v>150</v>
-      </c>
-      <c r="E49" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>83</v>
       </c>
       <c r="B50">
         <v>0.2</v>
       </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
       <c r="D50" t="s">
-        <v>150</v>
-      </c>
-      <c r="E50" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>84</v>
       </c>
       <c r="B51">
         <v>0.2</v>
       </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
       <c r="D51" t="s">
-        <v>150</v>
-      </c>
-      <c r="E51" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>85</v>
       </c>
       <c r="B52">
         <v>0.1</v>
       </c>
+      <c r="C52" t="s">
+        <v>150</v>
+      </c>
       <c r="D52" t="s">
-        <v>150</v>
-      </c>
-      <c r="E52" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>86</v>
       </c>
       <c r="B53">
         <v>0.15</v>
       </c>
+      <c r="C53" t="s">
+        <v>150</v>
+      </c>
       <c r="D53" t="s">
-        <v>150</v>
-      </c>
-      <c r="E53" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>87</v>
       </c>
       <c r="B54" s="3">
         <v>6.9999999999999999E-6</v>
       </c>
+      <c r="C54" t="s">
+        <v>150</v>
+      </c>
       <c r="D54" t="s">
-        <v>150</v>
-      </c>
-      <c r="E54" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>88</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
+      <c r="C55" t="s">
+        <v>151</v>
+      </c>
       <c r="D55" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>90</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
+      <c r="C56" t="s">
+        <v>151</v>
+      </c>
       <c r="D56" t="s">
-        <v>151</v>
-      </c>
-      <c r="E56" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>92</v>
       </c>
       <c r="B57">
         <v>4</v>
       </c>
+      <c r="C57" t="s">
+        <v>151</v>
+      </c>
       <c r="D57" t="s">
-        <v>151</v>
-      </c>
-      <c r="E57" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>94</v>
       </c>
       <c r="B58">
         <v>4</v>
       </c>
+      <c r="C58" t="s">
+        <v>151</v>
+      </c>
       <c r="D58" t="s">
-        <v>151</v>
-      </c>
-      <c r="E58" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>96</v>
       </c>
       <c r="B59">
         <v>4</v>
       </c>
+      <c r="C59" t="s">
+        <v>151</v>
+      </c>
       <c r="D59" t="s">
-        <v>151</v>
-      </c>
-      <c r="E59" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>98</v>
       </c>
       <c r="B60">
         <v>4</v>
       </c>
+      <c r="C60" t="s">
+        <v>151</v>
+      </c>
       <c r="D60" t="s">
-        <v>151</v>
-      </c>
-      <c r="E60" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>100</v>
       </c>
       <c r="B61">
         <v>6</v>
       </c>
+      <c r="C61" t="s">
+        <v>151</v>
+      </c>
       <c r="D61" t="s">
-        <v>151</v>
-      </c>
-      <c r="E61" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>102</v>
       </c>
       <c r="B62">
         <v>5</v>
       </c>
+      <c r="C62" t="s">
+        <v>151</v>
+      </c>
       <c r="D62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E62" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
       <c r="B63">
         <v>5.5</v>
       </c>
+      <c r="C63" t="s">
+        <v>152</v>
+      </c>
       <c r="D63" t="s">
-        <v>152</v>
-      </c>
-      <c r="E63" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>91</v>
       </c>
       <c r="B64">
         <v>5.5</v>
       </c>
+      <c r="C64" t="s">
+        <v>152</v>
+      </c>
       <c r="D64" t="s">
-        <v>152</v>
-      </c>
-      <c r="E64" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>93</v>
       </c>
       <c r="B65">
         <v>5.5</v>
       </c>
+      <c r="C65" t="s">
+        <v>152</v>
+      </c>
       <c r="D65" t="s">
-        <v>152</v>
-      </c>
-      <c r="E65" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>95</v>
       </c>
       <c r="B66">
-        <v>5.5</v>
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>152</v>
       </c>
       <c r="D66" t="s">
-        <v>152</v>
-      </c>
-      <c r="E66" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>97</v>
       </c>
       <c r="B67">
-        <v>5.5</v>
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>152</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
-      </c>
-      <c r="E67" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>99</v>
       </c>
       <c r="B68">
-        <v>5.5</v>
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>152</v>
       </c>
       <c r="D68" t="s">
-        <v>152</v>
-      </c>
-      <c r="E68" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>101</v>
       </c>
       <c r="B69">
         <v>7</v>
       </c>
+      <c r="C69" t="s">
+        <v>152</v>
+      </c>
       <c r="D69" t="s">
-        <v>152</v>
-      </c>
-      <c r="E69" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>103</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
+      <c r="C70" t="s">
+        <v>152</v>
+      </c>
       <c r="D70" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>104</v>
       </c>
       <c r="B71" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C71" t="s">
+        <v>162</v>
+      </c>
       <c r="D71" t="s">
-        <v>162</v>
-      </c>
-      <c r="E71" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>105</v>
       </c>
       <c r="B72" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C72" t="s">
+        <v>162</v>
+      </c>
       <c r="D72" t="s">
-        <v>162</v>
-      </c>
-      <c r="E72" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>106</v>
       </c>
       <c r="B73" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C73" t="s">
+        <v>162</v>
+      </c>
       <c r="D73" t="s">
-        <v>162</v>
-      </c>
-      <c r="E73" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>107</v>
       </c>
       <c r="B74" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C74" t="s">
+        <v>162</v>
+      </c>
       <c r="D74" t="s">
-        <v>162</v>
-      </c>
-      <c r="E74" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>108</v>
       </c>
       <c r="B75" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C75" t="s">
+        <v>162</v>
+      </c>
       <c r="D75" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>109</v>
       </c>
       <c r="B76" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C76" t="s">
+        <v>162</v>
+      </c>
       <c r="D76" t="s">
-        <v>162</v>
-      </c>
-      <c r="E76" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>110</v>
       </c>
       <c r="B77" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C77" t="s">
+        <v>162</v>
+      </c>
       <c r="D77" t="s">
-        <v>162</v>
-      </c>
-      <c r="E77" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>111</v>
       </c>
       <c r="B78" s="3">
         <v>1E-4</v>
       </c>
+      <c r="C78" t="s">
+        <v>162</v>
+      </c>
       <c r="D78" t="s">
-        <v>162</v>
-      </c>
-      <c r="E78" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>112</v>
       </c>
       <c r="B79" s="3">
         <v>5.0000000000000004E-6</v>
       </c>
+      <c r="C79" t="s">
+        <v>163</v>
+      </c>
       <c r="D79" t="s">
-        <v>163</v>
-      </c>
-      <c r="E79" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>113</v>
       </c>
       <c r="B80" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
+      <c r="C80" t="s">
+        <v>163</v>
+      </c>
       <c r="D80" t="s">
-        <v>163</v>
-      </c>
-      <c r="E80" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>114</v>
       </c>
       <c r="B81" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
+      <c r="C81" t="s">
+        <v>163</v>
+      </c>
       <c r="D81" t="s">
-        <v>163</v>
-      </c>
-      <c r="E81" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>115</v>
       </c>
       <c r="B82" s="3">
         <v>3.4999999999999999E-6</v>
       </c>
+      <c r="C82" t="s">
+        <v>163</v>
+      </c>
       <c r="D82" t="s">
-        <v>163</v>
-      </c>
-      <c r="E82" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>116</v>
       </c>
       <c r="B83">
         <v>1.8E-3</v>
       </c>
+      <c r="C83" t="s">
+        <v>164</v>
+      </c>
       <c r="D83" t="s">
-        <v>164</v>
-      </c>
-      <c r="E83" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>117</v>
       </c>
       <c r="B84" s="3">
         <v>2.08E-14</v>
       </c>
+      <c r="C84" t="s">
+        <v>165</v>
+      </c>
       <c r="D84" t="s">
-        <v>165</v>
-      </c>
-      <c r="E84" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>118</v>
       </c>
@@ -2867,163 +2866,163 @@
         <f>10^-9.25</f>
         <v>5.6234132519034889E-10</v>
       </c>
+      <c r="C85" t="s">
+        <v>165</v>
+      </c>
       <c r="D85" t="s">
-        <v>165</v>
-      </c>
-      <c r="E85" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>119</v>
       </c>
       <c r="B86" s="3">
         <v>4.9399999999999995E-7</v>
       </c>
+      <c r="C86" t="s">
+        <v>165</v>
+      </c>
       <c r="D86" t="s">
-        <v>165</v>
-      </c>
-      <c r="E86" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>120</v>
       </c>
       <c r="B87" s="3">
         <v>1.7399999999999999E-5</v>
       </c>
+      <c r="C87" t="s">
+        <v>165</v>
+      </c>
       <c r="D87" t="s">
-        <v>165</v>
-      </c>
-      <c r="E87" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>121</v>
       </c>
       <c r="B88" s="3">
         <v>1.3200000000000001E-5</v>
       </c>
+      <c r="C88" t="s">
+        <v>165</v>
+      </c>
       <c r="D88" t="s">
-        <v>165</v>
-      </c>
-      <c r="E88" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>122</v>
       </c>
       <c r="B89" s="3">
         <v>1.5E-5</v>
       </c>
+      <c r="C89" t="s">
+        <v>165</v>
+      </c>
       <c r="D89" t="s">
-        <v>165</v>
-      </c>
-      <c r="E89" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>123</v>
       </c>
       <c r="B90" s="3">
         <v>1.38E-5</v>
       </c>
+      <c r="C90" t="s">
+        <v>165</v>
+      </c>
       <c r="D90" t="s">
-        <v>165</v>
-      </c>
-      <c r="E90" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>124</v>
       </c>
       <c r="B91">
         <v>2.7099999999999999E-2</v>
       </c>
+      <c r="C91" t="s">
+        <v>172</v>
+      </c>
       <c r="D91" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E91" t="s">
-        <v>173</v>
-      </c>
-      <c r="F91" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>126</v>
       </c>
       <c r="B92">
         <v>1.16E-3</v>
       </c>
+      <c r="C92" t="s">
+        <v>172</v>
+      </c>
       <c r="D92" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E92" t="s">
-        <v>174</v>
-      </c>
-      <c r="F92" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>127</v>
       </c>
       <c r="B93" s="3">
         <v>7.3800000000000005E-4</v>
       </c>
+      <c r="C93" t="s">
+        <v>172</v>
+      </c>
       <c r="D93" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E93" t="s">
-        <v>175</v>
-      </c>
-      <c r="F93" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>128</v>
       </c>
       <c r="B94">
         <v>8.3144999999999997E-2</v>
       </c>
-      <c r="D94" t="s">
+      <c r="C94" t="s">
         <v>176</v>
       </c>
-      <c r="F94" t="s">
+      <c r="E94" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>131</v>
       </c>
       <c r="B95">
         <v>1.0129999999999999</v>
       </c>
-      <c r="D95" t="s">
+      <c r="C95" t="s">
         <v>177</v>
       </c>
-      <c r="F95" t="s">
+      <c r="E95" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>132</v>
       </c>
@@ -3031,97 +3030,97 @@
         <f>35+273.15</f>
         <v>308.14999999999998</v>
       </c>
-      <c r="D96" t="s">
+      <c r="C96" t="s">
         <v>178</v>
       </c>
-      <c r="F96" t="s">
+      <c r="E96" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>133</v>
       </c>
       <c r="B97">
         <v>5.57E-2</v>
       </c>
-      <c r="D97" t="s">
+      <c r="C97" t="s">
         <v>179</v>
       </c>
-      <c r="F97" t="s">
+      <c r="E97" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>134</v>
       </c>
       <c r="B98" s="3">
         <v>50000</v>
       </c>
+      <c r="C98" t="s">
+        <v>180</v>
+      </c>
       <c r="D98" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E98" t="s">
-        <v>181</v>
-      </c>
-      <c r="F98" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>135</v>
       </c>
       <c r="B99">
         <v>200</v>
       </c>
-      <c r="D99" t="s">
+      <c r="C99" t="s">
         <v>182</v>
       </c>
-      <c r="F99" t="s">
+      <c r="E99" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>137</v>
       </c>
       <c r="B100">
         <v>3400</v>
       </c>
-      <c r="D100" t="s">
+      <c r="C100" t="s">
         <v>183</v>
       </c>
-      <c r="F100" t="s">
+      <c r="E100" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>139</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
-      <c r="D101" t="s">
+      <c r="C101" t="s">
         <v>184</v>
       </c>
-      <c r="F101" t="s">
+      <c r="E101" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>140</v>
       </c>
       <c r="B102">
         <v>178.47</v>
       </c>
-      <c r="D102" t="s">
+      <c r="C102" t="s">
         <v>185</v>
       </c>
-      <c r="F102" t="s">
+      <c r="E102" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>